<commit_message>
Added var quotes, Implementation of video archive, modularization of page content
</commit_message>
<xml_diff>
--- a/docs/Zeitaufwand.xlsx
+++ b/docs/Zeitaufwand.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nr.</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Ersetzen der externen Bilder durch lokale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung variabler Zitate auf Indexseite, Implementierung eines Videoarchivs, Modularisierung von Seiteninhalt. </t>
   </si>
 </sst>
 </file>
@@ -413,14 +416,14 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="99.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -483,7 +486,15 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="B5" s="2">
+        <v>43112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -497,7 +508,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="str">
         <f>SUM(D2:D6) &amp; "h"</f>
-        <v>6,5h</v>
+        <v>10,5h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>